<commit_message>
inspire address harmonised postla code 08011
</commit_message>
<xml_diff>
--- a/sources/Inspire/harmonizer/BuildingInspireTaxonomy.xlsx
+++ b/sources/Inspire/harmonizer/BuildingInspireTaxonomy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jose/PycharmProjects/CR_BCN_sources_implementation/sources/Inspire/harmonizer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194495E3-8671-8A41-81F2-5E8C48FDD276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F6E827-6EBE-2444-8C4E-D7B6D3DF5DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16580" activeTab="1" xr2:uid="{B44D480E-B109-674B-AE60-9641A6C1D58D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16580" xr2:uid="{B44D480E-B109-674B-AE60-9641A6C1D58D}"/>
   </bookViews>
   <sheets>
     <sheet name="conditionOfConstruction" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>SOURCE</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -482,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CBECA8B-3B21-0A4E-B5B3-2187E5EB85D4}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -550,6 +553,14 @@
         <v>19</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -559,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4178169-C805-D043-B712-DA50C796F62A}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>